<commit_message>
adding log results of the experiment
</commit_message>
<xml_diff>
--- a/RestrictedEvents.xlsx
+++ b/RestrictedEvents.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19029"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21126"/>
   <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98509653-1E6E-497E-AEF5-EF01FB7659B6}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Trump</t>
   </si>
@@ -40,12 +41,15 @@
   </si>
   <si>
     <t>Election</t>
+  </si>
+  <si>
+    <t>Brexit</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -390,11 +394,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:A8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -437,6 +441,11 @@
         <v>6</v>
       </c>
     </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
update to new R version, moved from excel to csv file
</commit_message>
<xml_diff>
--- a/RestrictedEvents.xlsx
+++ b/RestrictedEvents.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98509653-1E6E-497E-AEF5-EF01FB7659B6}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B05989A3-F82C-432F-8174-152A14BB6BCD}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="990" yWindow="570" windowWidth="24030" windowHeight="14445" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>

</xml_diff>